<commit_message>
Update Cálculo de Média-LEIC.xlsx
</commit_message>
<xml_diff>
--- a/Cálculo de Média-LEIC.xlsx
+++ b/Cálculo de Média-LEIC.xlsx
@@ -173,7 +173,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="160" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -666,7 +666,7 @@
     <xf fontId="1" fillId="7" borderId="9" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="10" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="10" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="10" numFmtId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -688,7 +688,7 @@
     <xf fontId="1" fillId="8" borderId="8" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="13" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="13" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="13" numFmtId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -708,7 +708,7 @@
     <xf fontId="1" fillId="7" borderId="11" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="15" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="15" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="15" numFmtId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -848,7 +848,7 @@
     <xf fontId="1" fillId="16" borderId="5" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="9" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="2" fillId="0" borderId="9" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1783,11 +1783,11 @@
       </c>
       <c r="H8" s="20">
         <f>SUMPRODUCT(E8:E25,F8:F25)/SUM(IF(F8&gt;9,E8,0),IF(F9&gt;9,E9,0),IF(F10&gt;9,E10,0),IF(F11&gt;9,E11,0),IF(F12&gt;9,E12,0),IF(F13&gt;9,E13,0),IF(F14&gt;9,E14,0),IF(F15&gt;9,E15,0),IF(F16&gt;9,E16,0),IF(F17&gt;9,E17,0),IF(F18&gt;9,E18,0),IF(F19&gt;9,E19,0),IF(F20&gt;9,E20,0),IF(F21&gt;9,E21,0),IF(F22&gt;9,E22,0),IF(F23&gt;9,E23,0),IF(F24&gt;9,E24,0),IF(F25&gt;9,E25,0))</f>
-        <v>16.481481481481481</v>
+        <v>16.483870967741936</v>
       </c>
       <c r="I8" s="32" t="str">
         <f>CONCATENATE(COUNTA(F8:F25)," / ",SUM(COUNTA(F8:F25),COUNTBLANK(F8:F25)),CHAR(10)," Cadeiras")</f>
-        <v xml:space="preserve">14 / 18
+        <v xml:space="preserve">16 / 18
  Cadeiras</v>
       </c>
       <c r="J8" s="42"/>
@@ -2117,7 +2117,7 @@
       <c r="H15" s="31"/>
       <c r="I15" s="62" t="str">
         <f>CONCATENATE(SUM(IF(F8&gt;9,E8,0),IF(F9&gt;9,E9,0),IF(F10&gt;9,E10,0),IF(F11&gt;9,E11,0),IF(F12&gt;9,E12,0),IF(F13&gt;9,E13,0),IF(F14&gt;9,E14,0),IF(F15&gt;9,E15,0),IF(F16&gt;9,E16,0),IF(F17&gt;9,E17,0),IF(F18&gt;9,E18,0),IF(F19&gt;9,E19,0),IF(F20&gt;9,E20,0),IF(F21&gt;9,E21,0),IF(F22&gt;9,E22,0),IF(F23&gt;9,E23,0),IF(F24&gt;9,E24,0),IF(F25&gt;9,E25,0))," / ",SUM(E8:E25),CHAR(10)," Créditos")</f>
-        <v xml:space="preserve">81 / 105
+        <v xml:space="preserve">93 / 105
  Créditos</v>
       </c>
       <c r="J15" s="42"/>
@@ -2195,7 +2195,7 @@
       </c>
       <c r="N17" s="68">
         <f>SUM(SUMPRODUCT(N6:N15,O6:O15),SUMPRODUCT(E8:E25,F8:F25),SUMPRODUCT(E3:E5,F3:F5),(N3*O3))/N19</f>
-        <v>15.44</v>
+        <v>15.518518518518519</v>
       </c>
       <c r="Q17" s="69"/>
       <c r="R17" s="69"/>
@@ -2228,7 +2228,7 @@
       </c>
       <c r="N18" s="70">
         <f>COUNTA(O6:O15,F8:F25,F3:F5,O3)</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q18" s="69"/>
       <c r="R18" s="69"/>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="N19" s="72">
         <f>SUM(IF(O6&gt;9,N6,0),IF(O7&gt;9,N7,0),IF(O8&gt;9,N8,0),IF(O9&gt;9,N9,0),IF(O10&gt;9,N10,0),IF(O11&gt;9,N11,0),IF(O12&gt;9,N12,0),IF(O13&gt;9,N13,0),IF(O14&gt;9,N14,0),IF(O15&gt;9,N15,0),IF(F8&gt;9,E8,0),IF(F9&gt;9,E9,0),IF(F10&gt;9,E10,0),IF(F11&gt;9,E11,0),IF(F12&gt;9,E12,0),IF(F13&gt;9,E13,0),IF(F14&gt;9,E14,0),IF(F15&gt;9,E15,0),IF(F16&gt;9,E16,0),IF(F17&gt;9,E17,0),IF(F18&gt;9,E18,0),IF(F19&gt;9,E19,0),IF(F20&gt;9,E20,0),IF(F21&gt;9,E21,0),IF(F22&gt;9,E22,0),IF(F23&gt;9,E23,0),IF(F24&gt;9,E24,0),IF(F25&gt;9,E25,0),IF(F3&gt;9,E3,0),IF(F4&gt;9,E4,0),IF(F5&gt;9,E5,0), IF(O3&gt;9,N3,0))</f>
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="Q19" s="69"/>
       <c r="R19" s="69"/>
@@ -2405,10 +2405,12 @@
       <c r="E24" s="17">
         <v>6</v>
       </c>
-      <c r="F24" s="18"/>
-      <c r="G24" s="19" t="str">
+      <c r="F24" s="18">
+        <v>15</v>
+      </c>
+      <c r="G24" s="19">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0.5</v>
       </c>
       <c r="H24" s="31"/>
       <c r="I24" s="66"/>
@@ -2417,7 +2419,7 @@
       </c>
       <c r="N24" s="75">
         <f>N19/N23</f>
-        <v>0.83333333333333337</v>
+        <v>0.90000000000000002</v>
       </c>
       <c r="O24" s="69"/>
       <c r="P24" s="69"/>
@@ -2438,10 +2440,12 @@
       <c r="E25" s="23">
         <v>6</v>
       </c>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40" t="str">
+      <c r="F25" s="40">
+        <v>18</v>
+      </c>
+      <c r="G25" s="40">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0.59999999999999998</v>
       </c>
       <c r="H25" s="41"/>
       <c r="I25" s="78"/>

</xml_diff>